<commit_message>
update of peer feedback
</commit_message>
<xml_diff>
--- a/Beoordeling preliminary/9_10_preliminary_ML_report feedback_Jeroen_Koen_JaapJan_1462623.xlsx
+++ b/Beoordeling preliminary/9_10_preliminary_ML_report feedback_Jeroen_Koen_JaapJan_1462623.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koend\Documents\steenpapierschaar-tech\Beoordeling preliminary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjgroenendijk/school/steenpapierschaar-tech/Beoordeling preliminary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEEFC29-DC2C-4156-BDF8-709E07D49CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14489E79-68D8-0A4E-B698-A5876B7A925B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assessment form" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>Criteria</t>
   </si>
@@ -264,6 +264,21 @@
   </si>
   <si>
     <t>Pipline lijkt me logisch. Verder het uitleggen van de ML principes lijkt me niet van toepassing. Vertel kort wat je ondervonden hebt en de principes die echt iets uit maken.</t>
+  </si>
+  <si>
+    <t>Ja, functionele en techische vereisten zijn opgesomd en geprioriteerd. Bam, volle punten</t>
+  </si>
+  <si>
+    <t>Goed dat de leerdoelen erbij staan. Wellicht zijn de leerdoelen te combineren met de Problem Statement? Problem statement zou ook meer technische details mogen bevatten. Ik zie geen bijbehorende vraagstukken. Problem statement is niet specifiek en niet meetbaar. De requirements zijn wel specifiek gemaakt, dus problem statement moet ook wel gaan lukken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Of de dataset gemaakt is? Vast wel. Wat betreft de feature engineering ziet de teskt er goed, maar nog niet af uit. Zo missen de grafieken nog, maar hier wordt al aan gewerkt aan het commentaar in de documenten te zien. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dit kan ik niet terugvinden in de tekst. </t>
+  </si>
+  <si>
+    <t>Heel kort wordt dit toegelicht, maar het lijkt nog niet uitgewerkt te zijn in de tekst.</t>
   </si>
 </sst>
 </file>
@@ -630,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -770,6 +785,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,19 +806,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1074,35 +1095,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4255BA78-6A7E-4932-9D92-13E6845AA151}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.7109375" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="27"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>33</v>
       </c>
@@ -1113,7 +1134,7 @@
       <c r="D2" s="26"/>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>32</v>
       </c>
@@ -1124,7 +1145,7 @@
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>37</v>
       </c>
@@ -1135,8 +1156,8 @@
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>39</v>
       </c>
@@ -1151,12 +1172,12 @@
         <v>42</v>
       </c>
       <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+    <row r="9" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+      <c r="A9" s="54" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="29"/>
@@ -1172,12 +1193,14 @@
       <c r="F9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="39" t="s">
+        <v>56</v>
+      </c>
       <c r="H9" s="39"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="272.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
+    <row r="10" spans="1:9" ht="272.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="55"/>
       <c r="B10" s="30"/>
       <c r="C10" s="30">
         <v>3</v>
@@ -1191,12 +1214,14 @@
       <c r="F10" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="H10" s="39"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+    <row r="11" spans="1:9" ht="159.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="29"/>
@@ -1206,36 +1231,40 @@
       <c r="D11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="51" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="40"/>
+      <c r="G11" s="41" t="s">
+        <v>57</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="41"/>
     </row>
-    <row r="12" spans="1:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
+    <row r="12" spans="1:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="56"/>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="52" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="40"/>
+      <c r="G12" s="41" t="s">
+        <v>58</v>
+      </c>
       <c r="H12" s="40"/>
       <c r="I12" s="41"/>
     </row>
-    <row r="13" spans="1:9" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
+    <row r="13" spans="1:9" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="55"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30">
         <v>2</v>
@@ -1243,17 +1272,19 @@
       <c r="D13" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="53" t="s">
         <v>49</v>
       </c>
       <c r="F13" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="40"/>
+      <c r="G13" s="41" t="s">
+        <v>59</v>
+      </c>
       <c r="H13" s="40"/>
       <c r="I13" s="40"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>38</v>
       </c>
@@ -1281,17 +1312,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
@@ -1331,7 +1362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -1351,102 +1382,102 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="C4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="C7" s="13"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="C8" s="13"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="C9" s="13"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="C10" s="13"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
     </row>
   </sheetData>
@@ -1463,18 +1494,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" style="13" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="53.83203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="70.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +1525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
@@ -1514,7 +1545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
@@ -1554,115 +1585,115 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="23"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="23"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="23"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="23"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="23"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="24"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="25"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="25"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="25"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="25"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="25"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="25"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="25"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="25"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="25"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="25"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="25"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="23"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="25"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="25"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="25"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="25"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="25"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="25"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="25"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="25"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="25"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="25"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="23"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="25"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="23"/>
     </row>
   </sheetData>

</xml_diff>